<commit_message>
adicionando os campos de habilidade macro e micro vagas.com
</commit_message>
<xml_diff>
--- a/dicionario-skills.xlsx
+++ b/dicionario-skills.xlsx
@@ -4,11 +4,11 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Habilidades"/>
-    <sheet r:id="rId2" sheetId="2" name="Competências"/>
+    <sheet r:id="rId2" sheetId="2" name="Competencias"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">Habilidades!$A$1:$C$67</definedName>
@@ -616,7 +616,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -925,7 +925,7 @@
   </sheetPr>
   <dimension ref="A1:C1055"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6623,7 +6623,7 @@
   </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6631,7 +6631,7 @@
     <col min="2" max="2" style="3" width="54.71928571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6639,7 +6639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -6647,7 +6647,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -6655,7 +6655,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -6663,7 +6663,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -6671,7 +6671,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -6679,7 +6679,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -6687,7 +6687,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -6695,7 +6695,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -6703,7 +6703,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -6711,7 +6711,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -6719,7 +6719,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -6727,7 +6727,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -6735,7 +6735,7 @@
         <v>25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -6743,7 +6743,7 @@
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -6751,7 +6751,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>

</xml_diff>